<commit_message>
CLIPS with more files
</commit_message>
<xml_diff>
--- a/Lab5_ProdMod/Test.xlsx
+++ b/Lab5_ProdMod/Test.xlsx
@@ -26,7 +26,7 @@
     <x:t>f11=f9</x:t>
   </x:si>
   <x:si>
-    <x:t>ЕСЛИ t4, ТО t2</x:t>
+    <x:t>t4 -&gt; t2</x:t>
   </x:si>
   <x:si>
     <x:t>f2</x:t>
@@ -38,7 +38,7 @@
     <x:t>f12=f9</x:t>
   </x:si>
   <x:si>
-    <x:t>ЕСЛИ t5, ТО t2</x:t>
+    <x:t>t5 -&gt; t2</x:t>
   </x:si>
   <x:si>
     <x:t>f3</x:t>
@@ -50,7 +50,7 @@
     <x:t>f13=f10</x:t>
   </x:si>
   <x:si>
-    <x:t>ЕСЛИ t6, ТО t3</x:t>
+    <x:t>t6 -&gt; t3</x:t>
   </x:si>
   <x:si>
     <x:t>f4</x:t>
@@ -62,7 +62,7 @@
     <x:t>f14=f10</x:t>
   </x:si>
   <x:si>
-    <x:t>ЕСЛИ t7, ТО t3</x:t>
+    <x:t>t7 -&gt; t3</x:t>
   </x:si>
   <x:si>
     <x:t>f5</x:t>
@@ -74,7 +74,7 @@
     <x:t>f15=f11</x:t>
   </x:si>
   <x:si>
-    <x:t>ЕСЛИ t8, ТО t4</x:t>
+    <x:t>t8 -&gt; t4</x:t>
   </x:si>
   <x:si>
     <x:t>f6</x:t>
@@ -86,7 +86,7 @@
     <x:t>f10=f11</x:t>
   </x:si>
   <x:si>
-    <x:t>ЕСЛИ t3, ТО t4</x:t>
+    <x:t>t3 -&gt; t4</x:t>
   </x:si>
   <x:si>
     <x:t>f7</x:t>
@@ -98,7 +98,7 @@
     <x:t>f3=f12</x:t>
   </x:si>
   <x:si>
-    <x:t>ЕСЛИ c, ТО t5</x:t>
+    <x:t>c -&gt; t5</x:t>
   </x:si>
   <x:si>
     <x:t>f8</x:t>
@@ -110,7 +110,7 @@
     <x:t>f4=f12</x:t>
   </x:si>
   <x:si>
-    <x:t>ЕСЛИ d, ТО t5</x:t>
+    <x:t>d -&gt; t5</x:t>
   </x:si>
   <x:si>
     <x:t>f9</x:t>
@@ -122,7 +122,7 @@
     <x:t>f9&amp;f5=f13</x:t>
   </x:si>
   <x:si>
-    <x:t>ЕСЛИ t2, e, ТО t6</x:t>
+    <x:t>t2, e -&gt; t6</x:t>
   </x:si>
   <x:si>
     <x:t>f10</x:t>
@@ -134,7 +134,7 @@
     <x:t>f6=f14</x:t>
   </x:si>
   <x:si>
-    <x:t>ЕСЛИ f, ТО t7</x:t>
+    <x:t>f -&gt; t7</x:t>
   </x:si>
   <x:si>
     <x:t>f11</x:t>
@@ -146,7 +146,7 @@
     <x:t>f7=f14</x:t>
   </x:si>
   <x:si>
-    <x:t>ЕСЛИ g, ТО t7</x:t>
+    <x:t>g -&gt; t7</x:t>
   </x:si>
   <x:si>
     <x:t>f12</x:t>
@@ -158,7 +158,7 @@
     <x:t>f1&amp;f2=f15</x:t>
   </x:si>
   <x:si>
-    <x:t>ЕСЛИ a, b, ТО t8</x:t>
+    <x:t>a, b -&gt; t8</x:t>
   </x:si>
   <x:si>
     <x:t>f13</x:t>
@@ -170,7 +170,7 @@
     <x:t>f9&amp;f10=f8</x:t>
   </x:si>
   <x:si>
-    <x:t>ЕСЛИ t2, t3, ТО t1</x:t>
+    <x:t>t2, t3 -&gt; t1</x:t>
   </x:si>
   <x:si>
     <x:t>f14</x:t>

</xml_diff>